<commit_message>
BC Báo Cáo + Nhân sự
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Report/BaoCaoNhapHang/Teamplate_BaoCaoNhapHangTheoNhaCungCap.xlsx
+++ b/banhang24/Template/ExportExcel/Report/BaoCaoNhapHang/Teamplate_BaoCaoNhapHangTheoNhaCungCap.xlsx
@@ -17,10 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>Tổng cộng:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <r>
       <t xml:space="preserve">Điện thoại
@@ -192,7 +189,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -204,14 +201,8 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -235,30 +226,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -272,7 +239,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -287,7 +254,6 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -300,12 +266,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -321,16 +281,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -638,19 +592,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" style="15" customWidth="1"/>
-    <col min="3" max="3" width="38" style="10" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" style="12" customWidth="1"/>
+    <col min="3" max="3" width="38" style="9" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" style="9" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" style="5" customWidth="1"/>
     <col min="6" max="6" width="18" style="5" customWidth="1"/>
     <col min="7" max="7" width="16.42578125" style="5" customWidth="1"/>
@@ -660,75 +614,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+    </row>
+    <row r="4" spans="1:10" s="3" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="2"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-    </row>
-    <row r="4" spans="1:10" s="3" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="7" t="s">
+      <c r="C4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="D4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="F4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="G4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" s="9" t="s">
+      <c r="I4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="9" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -736,10 +690,10 @@
       <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
@@ -747,10 +701,10 @@
       <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -758,10 +712,10 @@
       <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
@@ -769,10 +723,10 @@
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -780,10 +734,10 @@
       <c r="I9" s="4"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -791,10 +745,10 @@
       <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -802,10 +756,10 @@
       <c r="I11" s="4"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
@@ -813,10 +767,10 @@
       <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
@@ -824,10 +778,10 @@
       <c r="I13" s="4"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
@@ -835,10 +789,10 @@
       <c r="I14" s="4"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
@@ -846,10 +800,10 @@
       <c r="I15" s="4"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
@@ -857,10 +811,10 @@
       <c r="I16" s="4"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
@@ -868,10 +822,10 @@
       <c r="I17" s="4"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
@@ -879,10 +833,10 @@
       <c r="I18" s="4"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
@@ -890,10 +844,10 @@
       <c r="I19" s="4"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
@@ -901,10 +855,10 @@
       <c r="I20" s="4"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
@@ -912,10 +866,10 @@
       <c r="I21" s="4"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
+      <c r="A22" s="10"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
@@ -923,10 +877,10 @@
       <c r="I22" s="4"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
+      <c r="A23" s="10"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
@@ -934,10 +888,10 @@
       <c r="I23" s="4"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
+      <c r="A24" s="10"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
@@ -945,10 +899,10 @@
       <c r="I24" s="4"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
+      <c r="A25" s="10"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
@@ -956,10 +910,10 @@
       <c r="I25" s="4"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
+      <c r="A26" s="10"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
@@ -967,10 +921,10 @@
       <c r="I26" s="4"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
+      <c r="A27" s="10"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
@@ -978,48 +932,19 @@
       <c r="I27" s="4"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
+      <c r="A28" s="10"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
     </row>
-    <row r="29" spans="1:9" s="6" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="11">
-        <f>SUM(E$5:E28)</f>
-        <v>0</v>
-      </c>
-      <c r="F29" s="11">
-        <f>SUM(F$5:F28)</f>
-        <v>0</v>
-      </c>
-      <c r="G29" s="11">
-        <f>SUM(G$5:G28)</f>
-        <v>0</v>
-      </c>
-      <c r="H29" s="11">
-        <f>SUM(H$5:H28)</f>
-        <v>0</v>
-      </c>
-      <c r="I29" s="11">
-        <f>SUM(I$5:I28)</f>
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A29:C29"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A3:I3"/>
   </mergeCells>

</xml_diff>